<commit_message>
First adaptation for ETEM acquisition. To be tested and recorrected for ESEM
</commit_message>
<xml_diff>
--- a/Functions.xlsx
+++ b/Functions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mon Drive\Travail\Doctorat\Projets\Process_Integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49137D4C-3EEF-4FED-ACDB-DD341D7E701C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FDA7FB-117D-410D-8735-F3C7DD09B6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{C305C823-4F13-49D0-98C4-00E6FB2EC8DA}"/>
+    <workbookView xWindow="14622" yWindow="3402" windowWidth="7110" windowHeight="5928" xr2:uid="{C305C823-4F13-49D0-98C4-00E6FB2EC8DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>Fonction</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>SetBeamBlanked()</t>
+  </si>
+  <si>
+    <t>SetMagIndex() ?</t>
+  </si>
+  <si>
+    <t>GetFocus()</t>
   </si>
 </sst>
 </file>
@@ -648,16 +654,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A015F2-1972-4E24-9C18-A1E31419C6F9}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="20.7890625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47.47265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="54.62890625" style="3" customWidth="1"/>
     <col min="3" max="3" width="38.47265625" style="3" customWidth="1"/>
     <col min="4" max="4" width="65.68359375" style="3" customWidth="1"/>
     <col min="5" max="16384" width="10.9453125" style="3"/>
@@ -879,49 +885,47 @@
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="2"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="2"/>
-      <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>56</v>
@@ -930,10 +934,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>56</v>
@@ -941,28 +945,32 @@
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="2"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="A31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="2"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="D33" s="4"/>
     </row>
@@ -970,97 +978,97 @@
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="2"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="2"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="A38" s="2"/>
+      <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="2"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="2"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="2"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="A42" s="2"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="2"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D44" s="4"/>
     </row>
@@ -1068,7 +1076,7 @@
       <c r="A45" s="2"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D45" s="4"/>
     </row>
@@ -1076,7 +1084,7 @@
       <c r="A46" s="2"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D46" s="4"/>
     </row>
@@ -1084,47 +1092,55 @@
       <c r="A47" s="2"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2"/>
       <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
+      <c r="C48" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="A49" s="2"/>
+      <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="2"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="2"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4" t="s">
+      <c r="B52" s="4"/>
+      <c r="C52" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="2"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
       <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="2"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>